<commit_message>
Authoration is ready Finish 3-commit
</commit_message>
<xml_diff>
--- a/src/main/resources/questions.xlsx
+++ b/src/main/resources/questions.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
   <si>
     <t>Id</t>
   </si>
@@ -94,6 +94,51 @@
   </si>
   <si>
     <t>9</t>
+  </si>
+  <si>
+    <t>___ you a student ?</t>
+  </si>
+  <si>
+    <t>Are</t>
+  </si>
+  <si>
+    <t>[Is, Do, Have]</t>
+  </si>
+  <si>
+    <t>Translate 'book' into Uzbek</t>
+  </si>
+  <si>
+    <t>kitob</t>
+  </si>
+  <si>
+    <t>[qalam, ruchka, daftar]</t>
+  </si>
+  <si>
+    <t>Translate 'apple' into Uzbek</t>
+  </si>
+  <si>
+    <t>olma</t>
+  </si>
+  <si>
+    <t>[gilos, olcha, anor]</t>
+  </si>
+  <si>
+    <t>Translate 'dog' into Uzbek</t>
+  </si>
+  <si>
+    <t>it</t>
+  </si>
+  <si>
+    <t>[mushik, tovuq, sichqon]</t>
+  </si>
+  <si>
+    <t>Translate 'cat' into Uzbek</t>
+  </si>
+  <si>
+    <t>mushuk</t>
+  </si>
+  <si>
+    <t>[it, sichqon, tovuq]</t>
   </si>
 </sst>
 </file>
@@ -311,17 +356,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="2.74609375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="3.26953125" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="9.85546875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="9.1875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="7.76171875" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="15.1953125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="25.85546875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="8.125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="23.0390625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -341,6 +386,91 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n" s="0">
+        <v>9.0</v>
+      </c>
+      <c r="B2" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n" s="0">
+        <v>10.0</v>
+      </c>
+      <c r="B3" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n" s="0">
+        <v>11.0</v>
+      </c>
+      <c r="B4" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n" s="0">
+        <v>12.0</v>
+      </c>
+      <c r="B5" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n" s="0">
+        <v>13.0</v>
+      </c>
+      <c r="B6" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>